<commit_message>
Added money to other(s) income
</commit_message>
<xml_diff>
--- a/UniversityExpenseTracker.xlsx
+++ b/UniversityExpenseTracker.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\University Expenses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UniversityExpenseTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5DE0CB-7B9A-4688-8909-0BA73DD762AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E972B8-882D-472C-9FA4-869366F70C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{FA22AA95-7C80-4231-8CA3-A075350F7AA4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Year1" sheetId="1" r:id="rId1"/>
+    <sheet name="Year2" sheetId="2" r:id="rId2"/>
+    <sheet name="Year3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="35">
   <si>
     <t>Student Finance</t>
   </si>
@@ -433,13 +435,13 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -770,7 +772,987 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E961D082-BBAD-424D-9BEC-0E43985F1FFF}">
   <dimension ref="A2:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="19.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="14.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="14.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="1" customWidth="1"/>
+    <col min="10" max="15" width="14.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="19.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="41">
+        <f>SUM(B4:B5)</f>
+        <v>9798</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="39">
+        <f>SUM(E4:E5)</f>
+        <v>7089</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="42"/>
+      <c r="D3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="40"/>
+      <c r="G3" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>9488</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>6867</v>
+      </c>
+      <c r="G4" s="7">
+        <f>B2-E2</f>
+        <v>2709</v>
+      </c>
+      <c r="I4" s="9">
+        <f>B10</f>
+        <v>64.5</v>
+      </c>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="6">
+        <v>310</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="6">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="O9" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="22"/>
+      <c r="B10" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="C10" s="11">
+        <f>B10</f>
+        <v>64.5</v>
+      </c>
+      <c r="D10" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="E10" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="F10" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="G10" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="H10" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="I10" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="J10" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="K10" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="L10" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="M10" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="N10" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="O10" s="6">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="11">
+        <f>B10-(B11+B12+B13+B14)</f>
+        <v>64.5</v>
+      </c>
+      <c r="C15" s="11">
+        <f>C10-(C11+C12+C13+C14)</f>
+        <v>64.5</v>
+      </c>
+      <c r="D15" s="11">
+        <f>D10-(D11+D12+D13+D14)</f>
+        <v>64.5</v>
+      </c>
+      <c r="E15" s="11">
+        <f>E10-(E11+E12+E13+E14)</f>
+        <v>64.5</v>
+      </c>
+      <c r="F15" s="11">
+        <f t="shared" ref="F15:O15" si="0">F10-(F11+F12+F13+F14)</f>
+        <v>64.5</v>
+      </c>
+      <c r="G15" s="11">
+        <f t="shared" si="0"/>
+        <v>64.5</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="0"/>
+        <v>64.5</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" si="0"/>
+        <v>64.5</v>
+      </c>
+      <c r="J15" s="11">
+        <f t="shared" si="0"/>
+        <v>64.5</v>
+      </c>
+      <c r="K15" s="11">
+        <f t="shared" si="0"/>
+        <v>64.5</v>
+      </c>
+      <c r="L15" s="11">
+        <f t="shared" si="0"/>
+        <v>64.5</v>
+      </c>
+      <c r="M15" s="11">
+        <f t="shared" si="0"/>
+        <v>64.5</v>
+      </c>
+      <c r="N15" s="11">
+        <f t="shared" si="0"/>
+        <v>64.5</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" si="0"/>
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O16" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="P16" s="34">
+        <f>SUM(B15:O15)</f>
+        <v>903</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="N18" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="O18" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="24"/>
+      <c r="B19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="C19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="D19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="E19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="F19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="G19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="H19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="I19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="J19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="K19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="L19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="M19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="N19" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="O19" s="6">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="11">
+        <f>B19-(B20+B21+B22+B23)</f>
+        <v>64.5</v>
+      </c>
+      <c r="C24" s="11">
+        <f t="shared" ref="C24:O24" si="1">C19-(C20+C21+C22+C23)</f>
+        <v>64.5</v>
+      </c>
+      <c r="D24" s="11">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="E24" s="11">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="G24" s="11">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="H24" s="11">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="I24" s="11">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="J24" s="11">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="K24" s="11">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="L24" s="11">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="M24" s="11">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="N24" s="11">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+      <c r="O24" s="4">
+        <f t="shared" si="1"/>
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O25" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" s="34">
+        <f>SUM(B24:O24)</f>
+        <v>903</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="N27" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="26"/>
+      <c r="B28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="C28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="D28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="E28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="F28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="G28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="H28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="I28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="J28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="K28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="L28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="M28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="N28" s="11">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+      <c r="O28" s="6">
+        <f>G4/42</f>
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="4"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="4"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="4"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="11">
+        <f>B28-(B29+B30+B31+B32)</f>
+        <v>64.5</v>
+      </c>
+      <c r="C33" s="11">
+        <f t="shared" ref="C33:N33" si="2">C28-(C29+C30+C31+C32)</f>
+        <v>64.5</v>
+      </c>
+      <c r="D33" s="11">
+        <f t="shared" si="2"/>
+        <v>64.5</v>
+      </c>
+      <c r="E33" s="11">
+        <f t="shared" si="2"/>
+        <v>64.5</v>
+      </c>
+      <c r="F33" s="11">
+        <f t="shared" si="2"/>
+        <v>64.5</v>
+      </c>
+      <c r="G33" s="11">
+        <f t="shared" si="2"/>
+        <v>64.5</v>
+      </c>
+      <c r="H33" s="11">
+        <f t="shared" si="2"/>
+        <v>64.5</v>
+      </c>
+      <c r="I33" s="11">
+        <f t="shared" si="2"/>
+        <v>64.5</v>
+      </c>
+      <c r="J33" s="11">
+        <f t="shared" si="2"/>
+        <v>64.5</v>
+      </c>
+      <c r="K33" s="11">
+        <f t="shared" si="2"/>
+        <v>64.5</v>
+      </c>
+      <c r="L33" s="11">
+        <f t="shared" si="2"/>
+        <v>64.5</v>
+      </c>
+      <c r="M33" s="11">
+        <f t="shared" si="2"/>
+        <v>64.5</v>
+      </c>
+      <c r="N33" s="11">
+        <f t="shared" si="2"/>
+        <v>64.5</v>
+      </c>
+      <c r="O33" s="4">
+        <f>K21:K2228-(O29+O30+O31+O32)</f>
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O34" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="P34" s="34">
+        <f>SUM(B33:O33)</f>
+        <v>903</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="38">
+        <f>SUM(P16,P25,P34)</f>
+        <v>2709</v>
+      </c>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+    </row>
+    <row r="37" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+    </row>
+    <row r="38" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35"/>
+    </row>
+    <row r="39" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="35"/>
+    </row>
+    <row r="40" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+    </row>
+    <row r="41" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="35"/>
+    </row>
+    <row r="42" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="K2:N4"/>
+    <mergeCell ref="D36:F42"/>
+    <mergeCell ref="G36:I42"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B2:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6AC8D8C-F4BC-4BD5-8049-A6FA72DC204D}">
+  <dimension ref="A2:P42"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -808,12 +1790,12 @@
       <c r="I2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
@@ -830,10 +1812,10 @@
       <c r="I3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -856,10 +1838,10 @@
         <f>B10</f>
         <v>57.11904761904762</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -1647,99 +2629,1079 @@
     <row r="36" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="36" t="s">
+      <c r="D36" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="37">
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="38">
         <f>SUM(P16,P25,P34)</f>
         <v>2398.9999999999991</v>
       </c>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
       <c r="J36" s="35"/>
       <c r="K36" s="35"/>
     </row>
     <row r="37" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
       <c r="J37" s="35"/>
       <c r="K37" s="35"/>
     </row>
     <row r="38" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
       <c r="J38" s="35"/>
       <c r="K38" s="35"/>
     </row>
     <row r="39" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
       <c r="J39" s="35"/>
       <c r="K39" s="35"/>
     </row>
     <row r="40" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
       <c r="J40" s="35"/>
       <c r="K40" s="35"/>
     </row>
     <row r="41" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
       <c r="J41" s="35"/>
       <c r="K41" s="35"/>
     </row>
     <row r="42" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
       <c r="J42" s="35"/>
       <c r="K42" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="K2:N4"/>
     <mergeCell ref="D36:F42"/>
     <mergeCell ref="G36:I42"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CE16D7-9241-46CC-9ED9-8C2A37686568}">
+  <dimension ref="A2:P42"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="19.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="14.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="14.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="1" customWidth="1"/>
+    <col min="10" max="15" width="14.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="19.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="41">
+        <f>SUM(B4:B5)</f>
+        <v>9488</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="39">
+        <f>SUM(E4:E5)</f>
+        <v>7089</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="42"/>
+      <c r="D3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="40"/>
+      <c r="G3" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>9488</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>6867</v>
+      </c>
+      <c r="G4" s="7">
+        <f>B2-E2</f>
+        <v>2399</v>
+      </c>
+      <c r="I4" s="9">
+        <f>B10</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="6">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="O9" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="22"/>
+      <c r="B10" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="C10" s="11">
+        <f>B10</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="D10" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="E10" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="F10" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="G10" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="H10" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="I10" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="J10" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="K10" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="L10" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="M10" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="N10" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="O10" s="6">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="11">
+        <f>B10-(B11+B12+B13+B14)</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="C15" s="11">
+        <f>C10-(C11+C12+C13+C14)</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="D15" s="11">
+        <f>D10-(D11+D12+D13+D14)</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="E15" s="11">
+        <f>E10-(E11+E12+E13+E14)</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="F15" s="11">
+        <f t="shared" ref="F15:O15" si="0">F10-(F11+F12+F13+F14)</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="G15" s="11">
+        <f t="shared" si="0"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="0"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" si="0"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="J15" s="11">
+        <f t="shared" si="0"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="K15" s="11">
+        <f t="shared" si="0"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="L15" s="11">
+        <f t="shared" si="0"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="M15" s="11">
+        <f t="shared" si="0"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="N15" s="11">
+        <f t="shared" si="0"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" si="0"/>
+        <v>57.11904761904762</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O16" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="P16" s="34">
+        <f>SUM(B15:O15)</f>
+        <v>799.6666666666664</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="N18" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="O18" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="24"/>
+      <c r="B19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="C19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="D19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="E19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="F19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="G19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="H19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="I19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="J19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="K19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="L19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="M19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="N19" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="O19" s="6">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="11">
+        <f>B19-(B20+B21+B22+B23)</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="C24" s="11">
+        <f t="shared" ref="C24:O24" si="1">C19-(C20+C21+C22+C23)</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="D24" s="11">
+        <f t="shared" si="1"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="E24" s="11">
+        <f t="shared" si="1"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" si="1"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="G24" s="11">
+        <f t="shared" si="1"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="H24" s="11">
+        <f t="shared" si="1"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="I24" s="11">
+        <f t="shared" si="1"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="J24" s="11">
+        <f t="shared" si="1"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="K24" s="11">
+        <f t="shared" si="1"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="L24" s="11">
+        <f t="shared" si="1"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="M24" s="11">
+        <f t="shared" si="1"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="N24" s="11">
+        <f t="shared" si="1"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="O24" s="4">
+        <f t="shared" si="1"/>
+        <v>57.11904761904762</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O25" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" s="34">
+        <f>SUM(B24:O24)</f>
+        <v>799.6666666666664</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="N27" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="26"/>
+      <c r="B28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="C28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="D28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="E28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="F28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="G28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="H28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="I28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="J28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="K28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="L28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="M28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="N28" s="11">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="O28" s="6">
+        <f>G4/42</f>
+        <v>57.11904761904762</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="4"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="4"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="4"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="11">
+        <f>B28-(B29+B30+B31+B32)</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="C33" s="11">
+        <f t="shared" ref="C33:N33" si="2">C28-(C29+C30+C31+C32)</f>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="D33" s="11">
+        <f t="shared" si="2"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="E33" s="11">
+        <f t="shared" si="2"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="F33" s="11">
+        <f t="shared" si="2"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="G33" s="11">
+        <f t="shared" si="2"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="H33" s="11">
+        <f t="shared" si="2"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="I33" s="11">
+        <f t="shared" si="2"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="J33" s="11">
+        <f t="shared" si="2"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="K33" s="11">
+        <f t="shared" si="2"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="L33" s="11">
+        <f t="shared" si="2"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="M33" s="11">
+        <f t="shared" si="2"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="N33" s="11">
+        <f t="shared" si="2"/>
+        <v>57.11904761904762</v>
+      </c>
+      <c r="O33" s="4">
+        <f>K21:K2228-(O29+O30+O31+O32)</f>
+        <v>57.11904761904762</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O34" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="P34" s="34">
+        <f>SUM(B33:O33)</f>
+        <v>799.6666666666664</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="38">
+        <f>SUM(P16,P25,P34)</f>
+        <v>2398.9999999999991</v>
+      </c>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+    </row>
+    <row r="37" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+    </row>
+    <row r="38" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35"/>
+    </row>
+    <row r="39" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="35"/>
+    </row>
+    <row r="40" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+    </row>
+    <row r="41" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="35"/>
+    </row>
+    <row r="42" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:B3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="K2:N4"/>
+    <mergeCell ref="D36:F42"/>
+    <mergeCell ref="G36:I42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>